<commit_message>
import excel done, without validation
</commit_message>
<xml_diff>
--- a/public/template/Template Import Quiz.xlsx
+++ b/public/template/Template Import Quiz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnoviandaru\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ruko\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E91771D-A7C7-4422-A642-054DE7BE7FD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326F1053-2D21-4E02-82CD-67A649EEAFDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9812BD8F-7B10-4053-ACDF-F2695D87EBDE}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="16">
-  <si>
-    <t>CATEGORY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>QUESTION</t>
   </si>
@@ -51,28 +48,7 @@
     <t>TRUE ANSWER</t>
   </si>
   <si>
-    <t>EXAMPLE</t>
-  </si>
-  <si>
-    <t>Kata</t>
-  </si>
-  <si>
-    <t>Tes</t>
-  </si>
-  <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
   </si>
 </sst>
 </file>
@@ -95,14 +71,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,11 +89,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
       </patternFill>
     </fill>
   </fills>
@@ -144,18 +116,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Accent5" xfId="2" builtinId="45"/>
+  <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -469,16 +439,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D346803-D8DC-48E3-9B04-CEFF407DF175}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="B1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
@@ -488,7 +458,7 @@
     <col min="9" max="9" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,40 +480,18 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H2" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{F0476B01-10B6-409B-AF3D-0695F191EEDC}">
+      <formula1>"A,B,C,D,E"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
tambah contoh pengisian import quiz
</commit_message>
<xml_diff>
--- a/public/template/Template Import Quiz.xlsx
+++ b/public/template/Template Import Quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ruko\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326F1053-2D21-4E02-82CD-67A649EEAFDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A17D70-DF9F-4C75-AA8D-8DC350698871}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9812BD8F-7B10-4053-ACDF-F2695D87EBDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="23">
   <si>
     <t>QUESTION</t>
   </si>
@@ -49,13 +49,58 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Diantara berikut ini yang bukan merupakan anggota girlband Blackpink adalah?</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Jennie Kim</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Jisso</t>
+  </si>
+  <si>
+    <t>Nancy</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +123,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,8 +150,14 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -115,17 +180,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="60% - Accent5" xfId="2" builtinId="48"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -439,26 +555,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D346803-D8DC-48E3-9B04-CEFF407DF175}">
-  <dimension ref="B1:H2"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="74.77734375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="17.21875" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,15 +599,161 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H2" s="2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="I6" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{F0476B01-10B6-409B-AF3D-0695F191EEDC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7" xr:uid="{F0476B01-10B6-409B-AF3D-0695F191EEDC}">
       <formula1>"A,B,C,D,E"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>